<commit_message>
refactor(scanner): fix PEP 8 violations and update  material nomenclature to 'Gold Filled'
Cleaned up code syntax and updated business logic for material naming.

Code Improvements (PEP 8):
- Expanded single-line `for` loops and `try/except` blocks to multi-line structures for better readability and debugging.
- Replaced bare `except:` with `except Exception:` to prevent capturing system interrupts (KeyboardInterrupt).

Business Logic Updates:
- Updated the "Acero Dorado" material label to "Acero Dorado (Gold Filled)" in both the AI prompt and the closed list options.
- Ensured consistency in "Gold Filled" spelling (two words).
</commit_message>
<xml_diff>
--- a/catalogo_kanela.xlsx
+++ b/catalogo_kanela.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Daisy Charm</t>
+          <t>Dije Flor Rosa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -506,40 +506,40 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>aleacion</t>
+          <t>Aleación</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>rosa</t>
+          <t>Rosa</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>Mujer</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>424.13</v>
+        <v>22.03</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['joyería', 'daisy', 'charm', 'flor', 'rosa', 'dorado']</t>
+          <t>['dije', 'flor', 'rosa', 'aleación', 'joyería', 'dorado']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Charm de flores con diseño de margarita en color rosa con detalles dorados.</t>
+          <t>Dije en forma de flor con detalles dorados en el centro y en los bordes.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Este charm de flores es perfecto para joyería personalizada. Con su diseño detallado y color rosa suave, se adapta a una variedad de estilos y ocasiones. El dorado añade un toque de elegancia y sofisticación.</t>
+          <t>Este adorable dije en forma de flor es perfecto para cualquier joyería. Con detalles dorados en el centro y en los bordes, este dije añade un toque de elegancia a cualquier collar o pulsera. El material aleación asegura un acabado duradero y resistente.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>daisy_charm.json</t>
+          <t>dije_flor_pink</t>
         </is>
       </c>
     </row>

</xml_diff>